<commit_message>
Fix publication date and add link
Publication date is the date of publication in CISO Assistant.
</commit_message>
<xml_diff>
--- a/tools/anssi/anssi-architectures-si-sensibles-dr.xlsx
+++ b/tools/anssi/anssi-architectures-si-sensibles-dr.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/anssi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA2C66E-83AE-7641-B343-FB5D01FFD023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF80506-2915-3F4C-9759-70485CBD1A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="-28140" windowWidth="50880" windowHeight="27980" activeTab="2" xr2:uid="{EAEC94CD-3B95-0444-8BA9-DD3B74A80109}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20700" xr2:uid="{EAEC94CD-3B95-0444-8BA9-DD3B74A80109}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
     <sheet name="req" sheetId="1" r:id="rId2"/>
     <sheet name="implementation_groups" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">req!$A$1:$G$85</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -133,527 +136,528 @@
     <t>urn:intuitem:risk:framework:anssi-architectures-si-sensibles-dr</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adopter une approche pragmatique pour construire rapidement un socle de sécurité, à coût contenu pour l’entité. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renforcer le niveau de sécurité par des adaptations pouvant être dimensionnantes. La robustesse ou les niveaux de sécurité de produits ou de services clés sont attestés par un tiers (certification/qualification). </t>
+  </si>
+  <si>
+    <t>Maîtriser pleinement les recommandations des étapes 1 et 2. Compléter par des recommandations adaptées au niveau de menace grâce à une analyse de risques.</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>Recommandations sur les architectures des systèmes d'information sensibles ou Diffusion Restreinte</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>Identifier les types de SI nécessaires</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Déterminer le régime de protection des informations sensibles </t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homologuer tout SI sensible avant sa mise en production </t>
+  </si>
+  <si>
+    <t>R05+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isoler physiquement le SI sensible et le SI usuel </t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloisonner physiquement le SI sensible et le SI usuel </t>
+  </si>
+  <si>
+    <t>R05-</t>
+  </si>
+  <si>
+    <t>Cloisonner logiquement les données sensibles au sein d'un SI sensible</t>
+  </si>
+  <si>
+    <t>R06</t>
+  </si>
+  <si>
+    <t>Appliquer le principe de défense en profondeur en cas de mutualisation de ressources</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>Cloisonner les annuaires sensible et usuel</t>
+  </si>
+  <si>
+    <t>R08</t>
+  </si>
+  <si>
+    <t>Définir une stratégie d'homologation pour chaque interconnexion de SI sensible</t>
+  </si>
+  <si>
+    <t>R09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sécuriser les interconnexions de SI DR </t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sécuriser les interconnexions de SI sensibles </t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtrer les flux des interconnexions de SI sensibles </t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Appliquer les recommandations de l'ANSSI relatives à  l'interconnexion d'un SI à Internet</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>Passerelle de classe 1 : mettre en oeuvre au moins un pare-feu qualifié</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>Passerelle de classe 1 : mettre en oeuvre au moins un dispositif de rupture de flux</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passerelle de classe 1 : mettre en oeuvre un système de détection </t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>Passerelle de classe 1 : faire porter les fonctions de sécurité par des dispositifs distincts</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>Interdire la navigation Web depuis les SI sensibles</t>
+  </si>
+  <si>
+    <t>R18-</t>
+  </si>
+  <si>
+    <t>Permettre la navigation Web depuis des postes de rebond</t>
+  </si>
+  <si>
+    <t>Permettre la navigation Web sans postes de rebond</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>Chiffrer les informations DR transférées via des SI de classe 0</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiffrer les informations sensibles transférées via des SI de classe 0 </t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>Interdire l'accés aux applications sensibles depuis les SI non homologués</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>Cloisonner l'infrastructure de mise à  disposition sur Internet d'informations sensibles</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maîtriser les interconnexions descendantes des SI de classe 2 </t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>N'autoriser que des protocoles de transfert vers le système d'échanges sécurisés</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>Système d'échanges sécurisés : restreindre les accès aux seuls utilisateurs autorisés</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>Système d'échanges sécurisés : authentifier les utilisateurs avec un compte non sensible</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>Système d'échanges sécurisés : analyser le contenu des données échangées</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>Système d'échanges sécurisés : journaliser et imputer des données échangées</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>Recourir à des prestataires de services SSI disposant d'un visa de sécurité ANSSI</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquérir des produits de sécurité disposant d'un visa de sécurité ANSSI </t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>Respecter les conditions d'emploi des équipements de sécurité agréés</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>Cloisonner le SI sensible en zones ayant des niveaux de sécurité homogènes</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>Éviter l'installation de moyens informatiques sensibles dans les zones ouvertes au public</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloquer les communications latérales </t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>Durcir la configuration des matériels et des logiciels utilisés sur les SI sensibles</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marquer les informations sensibles </t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marquer les supports stockant des informations sensibles </t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adopter un code couleur pour le câblage des équipements </t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>Activer une authentification initiale forte</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protéger les secrets d'authentification </t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>Gérer avec rigueur l'affectation des droits d'accès logiques des comptes informatiques</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>Protéger le SI sensible des codes malveillants</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>Adapter la politique de protection contre les codes malveillants</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>Déployer des outils révèlant des activités suspectes</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>Supports amovibles : limiter leur usage au strict besoin opérationnel</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports amovibles : maîtriser leur gestion et leurs conditions d'usage </t>
+  </si>
+  <si>
+    <t>R47</t>
+  </si>
+  <si>
+    <t>Supports amovibles : privilégier l'utilisation de supports en lecture seule</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>Supports amovibles : utiliser des solutions de dépollution des supports de stockage</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>Maîtriser les moyens informatiques affectés aux utilisateurs d'un SI sensible</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connecter les ressources sensibles sur un réseau physique dédié </t>
+  </si>
+  <si>
+    <t>R50-</t>
+  </si>
+  <si>
+    <t>Connecter les ressources sensibles sur un réseau logique dédié</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authentifier les ressources sensibles vis-à -vis du réseau </t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>Utiliser un poste utilisateur sensible dédié</t>
+  </si>
+  <si>
+    <t>R52-</t>
+  </si>
+  <si>
+    <t>Utiliser un poste utilisateur multiniveau</t>
+  </si>
+  <si>
+    <t>Utiliser un poste utilisateur sensible avec accès distant au SI usuel</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>Appliquer les recommandations de l'ANSSI relatives au nomadisme numérique</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protéger physiquement les équipements d'accès nomade </t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sécuriser les canaux d'interconnexion nomades des SI DR </t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sécuriser les canaux d'interconnexion nomades des SI sensibles </t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>Chiffrer les données DR stockées sur des supports amovibles</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>Chiffrer les données sensibles stockées sur des supports amovibles</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>Chiffrer les flux réseau d'un équipement d'accès nomade sensible en toute circonstance</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>Mettre en place une architecture de réseau sans fil cloisonnée du SI sensible</t>
+  </si>
+  <si>
+    <t>R61</t>
+  </si>
+  <si>
+    <t>Bloquer l'accès aux portails captifs publics depuis des équipements d'accès nomades sensibles</t>
+  </si>
+  <si>
+    <t>R62</t>
+  </si>
+  <si>
+    <t>Appliquer les recommandations de l'ANSSI relatives à  l'administration sécurisée des SI</t>
+  </si>
+  <si>
+    <t>R63</t>
+  </si>
+  <si>
+    <t>Gérer les administrateurs d'un SI sensible</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>Sécuriser la chaîne de connexion pour l'administration à distance</t>
+  </si>
+  <si>
+    <t>R64-</t>
+  </si>
+  <si>
+    <t>Maîtriser les systèmes de télémaintenance connectés à des SI sensibles</t>
+  </si>
+  <si>
+    <t>R65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Définir et appliquer une politique de MCS </t>
+  </si>
+  <si>
+    <t>R66</t>
+  </si>
+  <si>
+    <t>Isoler les systèmes obsolètes</t>
+  </si>
+  <si>
+    <t>R67</t>
+  </si>
+  <si>
+    <t>Appliquer les recommandations de l'ANSSI relatives à  la journalisation</t>
+  </si>
+  <si>
+    <t>R68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conserver les journaux d'un SI sensible pendant 12 mois </t>
+  </si>
+  <si>
+    <t>R69</t>
+  </si>
+  <si>
+    <t>Recourir aux services d'un prestataire qualifié pour la supervision de sécurité</t>
+  </si>
+  <si>
+    <t>R70</t>
+  </si>
+  <si>
+    <t>Formaliser une procédure de déclaration des incidents de sécurité à l'ANSSI</t>
+  </si>
+  <si>
+    <t>R18--</t>
+  </si>
+  <si>
+    <t>R52--</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>Trier le patrimoine informationnel par niveau de sensibilité</t>
+  </si>
+  <si>
+    <t>Passerelle de classe 1 : mettre en oeuvre des taps qualifiés passifs</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Typologies de SI sensibles</t>
+  </si>
+  <si>
+    <t>Systèmes d'information (SI) non classifiés</t>
+  </si>
+  <si>
+    <t>Interconnexions directes de SI sensibles</t>
+  </si>
+  <si>
+    <t>Sécurisation au sein des SI sensibles</t>
+  </si>
+  <si>
+    <t>Sécurisation des postes de travail sensibles</t>
+  </si>
+  <si>
+    <t>Administration des SI sensibles</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>l1</t>
+  </si>
+  <si>
+    <t>l2</t>
+  </si>
+  <si>
+    <t>l3</t>
+  </si>
+  <si>
     <t>Outil d'aide et de suivi d'implémentation de la sécurité (OASIS)
-Recommandations sur les architectures des systèmes d'information sensibles ou Diffusion Restreinte</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adopter une approche pragmatique pour construire rapidement un socle de sécurité, à coût contenu pour l’entité. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renforcer le niveau de sécurité par des adaptations pouvant être dimensionnantes. La robustesse ou les niveaux de sécurité de produits ou de services clés sont attestés par un tiers (certification/qualification). </t>
-  </si>
-  <si>
-    <t>Maîtriser pleinement les recommandations des étapes 1 et 2. Compléter par des recommandations adaptées au niveau de menace grâce à une analyse de risques.</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>Recommandations sur les architectures des systèmes d'information sensibles ou Diffusion Restreinte</t>
-  </si>
-  <si>
-    <t>R02</t>
-  </si>
-  <si>
-    <t>Identifier les types de SI nécessaires</t>
-  </si>
-  <si>
-    <t>R03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déterminer le régime de protection des informations sensibles </t>
-  </si>
-  <si>
-    <t>R04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homologuer tout SI sensible avant sa mise en production </t>
-  </si>
-  <si>
-    <t>R05+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isoler physiquement le SI sensible et le SI usuel </t>
-  </si>
-  <si>
-    <t>R05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloisonner physiquement le SI sensible et le SI usuel </t>
-  </si>
-  <si>
-    <t>R05-</t>
-  </si>
-  <si>
-    <t>Cloisonner logiquement les données sensibles au sein d'un SI sensible</t>
-  </si>
-  <si>
-    <t>R06</t>
-  </si>
-  <si>
-    <t>Appliquer le principe de défense en profondeur en cas de mutualisation de ressources</t>
-  </si>
-  <si>
-    <t>R07</t>
-  </si>
-  <si>
-    <t>Cloisonner les annuaires sensible et usuel</t>
-  </si>
-  <si>
-    <t>R08</t>
-  </si>
-  <si>
-    <t>Définir une stratégie d'homologation pour chaque interconnexion de SI sensible</t>
-  </si>
-  <si>
-    <t>R09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sécuriser les interconnexions de SI DR </t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sécuriser les interconnexions de SI sensibles </t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filtrer les flux des interconnexions de SI sensibles </t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>Appliquer les recommandations de l'ANSSI relatives à  l'interconnexion d'un SI à Internet</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>Passerelle de classe 1 : mettre en oeuvre au moins un pare-feu qualifié</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>Passerelle de classe 1 : mettre en oeuvre au moins un dispositif de rupture de flux</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Passerelle de classe 1 : mettre en oeuvre un système de détection </t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>Passerelle de classe 1 : faire porter les fonctions de sécurité par des dispositifs distincts</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>Interdire la navigation Web depuis les SI sensibles</t>
-  </si>
-  <si>
-    <t>R18-</t>
-  </si>
-  <si>
-    <t>Permettre la navigation Web depuis des postes de rebond</t>
-  </si>
-  <si>
-    <t>Permettre la navigation Web sans postes de rebond</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>Chiffrer les informations DR transférées via des SI de classe 0</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chiffrer les informations sensibles transférées via des SI de classe 0 </t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>Interdire l'accés aux applications sensibles depuis les SI non homologués</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>Cloisonner l'infrastructure de mise à  disposition sur Internet d'informations sensibles</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maîtriser les interconnexions descendantes des SI de classe 2 </t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>N'autoriser que des protocoles de transfert vers le système d'échanges sécurisés</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>Système d'échanges sécurisés : restreindre les accès aux seuls utilisateurs autorisés</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>Système d'échanges sécurisés : authentifier les utilisateurs avec un compte non sensible</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>Système d'échanges sécurisés : analyser le contenu des données échangées</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>Système d'échanges sécurisés : journaliser et imputer des données échangées</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>Recourir à des prestataires de services SSI disposant d'un visa de sécurité ANSSI</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acquérir des produits de sécurité disposant d'un visa de sécurité ANSSI </t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>Respecter les conditions d'emploi des équipements de sécurité agréés</t>
-  </si>
-  <si>
-    <t>R32</t>
-  </si>
-  <si>
-    <t>Cloisonner le SI sensible en zones ayant des niveaux de sécurité homogènes</t>
-  </si>
-  <si>
-    <t>R33</t>
-  </si>
-  <si>
-    <t>Éviter l'installation de moyens informatiques sensibles dans les zones ouvertes au public</t>
-  </si>
-  <si>
-    <t>R34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bloquer les communications latérales </t>
-  </si>
-  <si>
-    <t>R35</t>
-  </si>
-  <si>
-    <t>Durcir la configuration des matériels et des logiciels utilisés sur les SI sensibles</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marquer les informations sensibles </t>
-  </si>
-  <si>
-    <t>R37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marquer les supports stockant des informations sensibles </t>
-  </si>
-  <si>
-    <t>R38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adopter un code couleur pour le câblage des équipements </t>
-  </si>
-  <si>
-    <t>R39</t>
-  </si>
-  <si>
-    <t>Activer une authentification initiale forte</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protéger les secrets d'authentification </t>
-  </si>
-  <si>
-    <t>R41</t>
-  </si>
-  <si>
-    <t>Gérer avec rigueur l'affectation des droits d'accès logiques des comptes informatiques</t>
-  </si>
-  <si>
-    <t>R42</t>
-  </si>
-  <si>
-    <t>Protéger le SI sensible des codes malveillants</t>
-  </si>
-  <si>
-    <t>R43</t>
-  </si>
-  <si>
-    <t>Adapter la politique de protection contre les codes malveillants</t>
-  </si>
-  <si>
-    <t>R44</t>
-  </si>
-  <si>
-    <t>Déployer des outils révèlant des activités suspectes</t>
-  </si>
-  <si>
-    <t>R45</t>
-  </si>
-  <si>
-    <t>Supports amovibles : limiter leur usage au strict besoin opérationnel</t>
-  </si>
-  <si>
-    <t>R46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports amovibles : maîtriser leur gestion et leurs conditions d'usage </t>
-  </si>
-  <si>
-    <t>R47</t>
-  </si>
-  <si>
-    <t>Supports amovibles : privilégier l'utilisation de supports en lecture seule</t>
-  </si>
-  <si>
-    <t>R48</t>
-  </si>
-  <si>
-    <t>Supports amovibles : utiliser des solutions de dépollution des supports de stockage</t>
-  </si>
-  <si>
-    <t>R49</t>
-  </si>
-  <si>
-    <t>Maîtriser les moyens informatiques affectés aux utilisateurs d'un SI sensible</t>
-  </si>
-  <si>
-    <t>R50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connecter les ressources sensibles sur un réseau physique dédié </t>
-  </si>
-  <si>
-    <t>R50-</t>
-  </si>
-  <si>
-    <t>Connecter les ressources sensibles sur un réseau logique dédié</t>
-  </si>
-  <si>
-    <t>R51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authentifier les ressources sensibles vis-à -vis du réseau </t>
-  </si>
-  <si>
-    <t>R52</t>
-  </si>
-  <si>
-    <t>Utiliser un poste utilisateur sensible dédié</t>
-  </si>
-  <si>
-    <t>R52-</t>
-  </si>
-  <si>
-    <t>Utiliser un poste utilisateur multiniveau</t>
-  </si>
-  <si>
-    <t>Utiliser un poste utilisateur sensible avec accès distant au SI usuel</t>
-  </si>
-  <si>
-    <t>R53</t>
-  </si>
-  <si>
-    <t>Appliquer les recommandations de l'ANSSI relatives au nomadisme numérique</t>
-  </si>
-  <si>
-    <t>R54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protéger physiquement les équipements d'accès nomade </t>
-  </si>
-  <si>
-    <t>R55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sécuriser les canaux d'interconnexion nomades des SI DR </t>
-  </si>
-  <si>
-    <t>R56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sécuriser les canaux d'interconnexion nomades des SI sensibles </t>
-  </si>
-  <si>
-    <t>R57</t>
-  </si>
-  <si>
-    <t>Chiffrer les données DR stockées sur des supports amovibles</t>
-  </si>
-  <si>
-    <t>R58</t>
-  </si>
-  <si>
-    <t>Chiffrer les données sensibles stockées sur des supports amovibles</t>
-  </si>
-  <si>
-    <t>R59</t>
-  </si>
-  <si>
-    <t>Chiffrer les flux réseau d'un équipement d'accès nomade sensible en toute circonstance</t>
-  </si>
-  <si>
-    <t>R60</t>
-  </si>
-  <si>
-    <t>Mettre en place une architecture de réseau sans fil cloisonnée du SI sensible</t>
-  </si>
-  <si>
-    <t>R61</t>
-  </si>
-  <si>
-    <t>Bloquer l'accès aux portails captifs publics depuis des équipements d'accès nomades sensibles</t>
-  </si>
-  <si>
-    <t>R62</t>
-  </si>
-  <si>
-    <t>Appliquer les recommandations de l'ANSSI relatives à  l'administration sécurisée des SI</t>
-  </si>
-  <si>
-    <t>R63</t>
-  </si>
-  <si>
-    <t>Gérer les administrateurs d'un SI sensible</t>
-  </si>
-  <si>
-    <t>R64</t>
-  </si>
-  <si>
-    <t>Sécuriser la chaîne de connexion pour l'administration à distance</t>
-  </si>
-  <si>
-    <t>R64-</t>
-  </si>
-  <si>
-    <t>Maîtriser les systèmes de télémaintenance connectés à des SI sensibles</t>
-  </si>
-  <si>
-    <t>R65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Définir et appliquer une politique de MCS </t>
-  </si>
-  <si>
-    <t>R66</t>
-  </si>
-  <si>
-    <t>Isoler les systèmes obsolètes</t>
-  </si>
-  <si>
-    <t>R67</t>
-  </si>
-  <si>
-    <t>Appliquer les recommandations de l'ANSSI relatives à  la journalisation</t>
-  </si>
-  <si>
-    <t>R68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conserver les journaux d'un SI sensible pendant 12 mois </t>
-  </si>
-  <si>
-    <t>R69</t>
-  </si>
-  <si>
-    <t>Recourir aux services d'un prestataire qualifié pour la supervision de sécurité</t>
-  </si>
-  <si>
-    <t>R70</t>
-  </si>
-  <si>
-    <t>Formaliser une procédure de déclaration des incidents de sécurité à l'ANSSI</t>
-  </si>
-  <si>
-    <t>R18--</t>
-  </si>
-  <si>
-    <t>R52--</t>
-  </si>
-  <si>
-    <t>R01</t>
-  </si>
-  <si>
-    <t>Trier le patrimoine informationnel par niveau de sensibilité</t>
-  </si>
-  <si>
-    <t>Passerelle de classe 1 : mettre en oeuvre des taps qualifiés passifs</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Typologies de SI sensibles</t>
-  </si>
-  <si>
-    <t>Systèmes d'information (SI) non classifiés</t>
-  </si>
-  <si>
-    <t>Interconnexions directes de SI sensibles</t>
-  </si>
-  <si>
-    <t>Sécurisation au sein des SI sensibles</t>
-  </si>
-  <si>
-    <t>Sécurisation des postes de travail sensibles</t>
-  </si>
-  <si>
-    <t>Administration des SI sensibles</t>
-  </si>
-  <si>
-    <t>lb</t>
-  </si>
-  <si>
-    <t>l1</t>
-  </si>
-  <si>
-    <t>l2</t>
-  </si>
-  <si>
-    <t>l3</t>
+Recommandations sur les architectures des systèmes d'information sensibles ou Diffusion Restreinte
+https://cyber.gouv.fr/publications/recommandations-pour-les-architectures-des-si-sensibles-ou-dr</t>
   </si>
 </sst>
 </file>
@@ -1146,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445255F7-0E18-1146-BE8F-C90E6402101B}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="242" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="242" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1178,7 +1182,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="8">
-        <v>45446</v>
+        <v>45677</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1202,15 +1206,15 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1258,15 +1262,15 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1299,10 +1303,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D58A10-8E07-794C-8BE7-D56F6849796F}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView zoomScale="191" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="12">
         <v>1</v>
@@ -1347,80 +1352,80 @@
         <v>2</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" s="10">
         <v>2</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="10">
         <v>2</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" s="10">
         <v>2</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="10">
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D6" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10">
         <v>1</v>
       </c>
@@ -1429,95 +1434,95 @@
         <v>3</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" s="10">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" s="10">
         <v>2</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D11" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="10">
         <v>2</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D12" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" s="10">
         <v>1</v>
       </c>
@@ -1526,401 +1531,401 @@
         <v>4</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B14" s="10">
         <v>2</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D14" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15" s="10">
         <v>2</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D15" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B16" s="10">
         <v>2</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D16" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B17" s="10">
         <v>2</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D17" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="10">
         <v>2</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D18" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19" s="10">
         <v>2</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D19" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B20" s="10">
         <v>2</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B21" s="10">
         <v>2</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D21" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B22" s="10">
         <v>2</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B23" s="10">
         <v>2</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D23" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B24" s="10">
         <v>2</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D24" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B25" s="10">
         <v>2</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D25" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B26" s="10">
         <v>2</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B27" s="10">
         <v>2</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D27" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B28" s="10">
         <v>2</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D28" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B29" s="10">
         <v>2</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D29" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B30" s="10">
         <v>2</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D30" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B31" s="10">
         <v>2</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D31" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B32" s="10">
         <v>2</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D32" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B33" s="10">
         <v>2</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B34" s="10">
         <v>2</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D34" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B35" s="10">
         <v>2</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D35" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B36" s="10">
         <v>2</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D36" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" s="10">
         <v>1</v>
       </c>
@@ -1929,350 +1934,350 @@
         <v>5</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B38" s="10">
         <v>2</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D38" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B39" s="10">
         <v>2</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D39" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B40" s="10">
         <v>2</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D40" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B41" s="10">
         <v>2</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D41" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B42" s="10">
         <v>2</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D42" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B43" s="10">
         <v>2</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D43" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B44" s="10">
         <v>2</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D44" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B45" s="10">
         <v>2</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D45" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B46" s="10">
         <v>2</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D46" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B47" s="10">
         <v>2</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D47" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B48" s="10">
         <v>2</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D48" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B49" s="10">
         <v>2</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D49" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B50" s="10">
         <v>2</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D50" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B51" s="10">
         <v>2</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D51" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B52" s="10">
         <v>2</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D52" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B53" s="10">
         <v>2</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D53" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B54" s="10">
         <v>2</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D54" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B55" s="10">
         <v>2</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D55" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B56" s="10">
         <v>2</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D56" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B57" s="10">
         <v>2</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D57" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" s="10">
         <v>1</v>
       </c>
@@ -2281,282 +2286,282 @@
         <v>6</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B59" s="10">
         <v>2</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D59" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B60" s="10">
         <v>2</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D60" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B61" s="10">
         <v>2</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D61" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B62" s="10">
         <v>2</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D62" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B63" s="10">
         <v>2</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D63" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B64" s="10">
         <v>2</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D64" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B65" s="10">
         <v>2</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B66" s="10">
         <v>2</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D66" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B67" s="10">
         <v>2</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D67" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B68" s="10">
         <v>2</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D68" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B69" s="10">
         <v>2</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D69" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B70" s="10">
         <v>2</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D70" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B71" s="10">
         <v>2</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D71" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B72" s="10">
         <v>2</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D72" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B73" s="10">
         <v>2</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D73" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B74" s="10">
         <v>2</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D74" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" s="10">
         <v>1</v>
       </c>
@@ -2565,180 +2570,187 @@
         <v>7</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B76" s="10">
         <v>2</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D76" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B77" s="10">
         <v>2</v>
       </c>
       <c r="C77" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D77" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B78" s="10">
         <v>2</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D78" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B79" s="10">
         <v>2</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D79" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B80" s="10">
         <v>2</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D80" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B81" s="10">
         <v>2</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D81" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B82" s="10">
         <v>2</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D82" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B83" s="10">
         <v>2</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D83" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B84" s="10">
         <v>2</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D84" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B85" s="10">
         <v>2</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D85" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>188</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G85" xr:uid="{62D58A10-8E07-794C-8BE7-D56F6849796F}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2747,7 +2759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B6C933-8B46-444C-ACAD-02A4AC9257EE}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2772,46 +2784,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>